<commit_message>
Teermino cargar datos de Excel
</commit_message>
<xml_diff>
--- a/src/main/java/Main/Libro1.xlsx
+++ b/src/main/java/Main/Libro1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facua\Desktop\TP DDS\2022-mi-no-mino-grupo-07\src\main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facua\Desktop\TP DDS\2022-mi-no-mino-grupo-07\src\main\java\Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9159F18-5F37-4762-BB7D-E98A5B335014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB33463-676A-4073-A586-1A0BB035A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51510C4E-3AE2-48E9-8511-FB6034014CB4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Actividad</t>
   </si>
@@ -55,46 +55,70 @@
     <t>Periodo de imputacion</t>
   </si>
   <si>
+    <t>Alcance</t>
+  </si>
+  <si>
     <t>Combustion fija</t>
   </si>
   <si>
     <t>Gas Natural</t>
   </si>
   <si>
-    <t>Diesel/Gasoil</t>
-  </si>
-  <si>
-    <t>Kerosene</t>
-  </si>
-  <si>
-    <t>Fuel Oil</t>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>Mensual</t>
+  </si>
+  <si>
+    <t>02/2020</t>
+  </si>
+  <si>
+    <t>Combustion movil</t>
+  </si>
+  <si>
+    <t>Combustible consumido - Gasoil</t>
+  </si>
+  <si>
+    <t>lts</t>
+  </si>
+  <si>
+    <t>Anual</t>
+  </si>
+  <si>
+    <t>/2021</t>
+  </si>
+  <si>
+    <t>Electricidad adquirida y consumida</t>
+  </si>
+  <si>
+    <t>Electricidad</t>
+  </si>
+  <si>
+    <t>Kwh</t>
+  </si>
+  <si>
+    <t>/2421</t>
   </si>
   <si>
     <t>Nafta</t>
   </si>
   <si>
-    <t>Carbon</t>
-  </si>
-  <si>
-    <t>Carbon de lenia</t>
-  </si>
-  <si>
-    <t>Lenia</t>
-  </si>
-  <si>
-    <t>Combustible consumido - Gasoil</t>
-  </si>
-  <si>
-    <t>Combustible consumido - GNC</t>
-  </si>
-  <si>
-    <t>Combustible consumido - Nafta</t>
-  </si>
-  <si>
-    <t>Electricidad</t>
-  </si>
-  <si>
-    <t>ma</t>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>Materia prima</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Logistica de productos y residuos</t>
+  </si>
+  <si>
+    <t>02/2026</t>
+  </si>
+  <si>
+    <t>Camion de carga</t>
   </si>
 </sst>
 </file>
@@ -130,8 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,15 +474,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D9F111-2FA5-45E2-8986-F34D78041A6B}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,81 +499,154 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="G7" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
datos de actividad resuelto
</commit_message>
<xml_diff>
--- a/src/main/java/Main/Libro1.xlsx
+++ b/src/main/java/Main/Libro1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facua\Desktop\TP DDS\2022-mi-no-mino-grupo-07\src\main\java\Main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NACHO\Desktop\TP DDS\2022-mi-no-mino-grupo-07\src\main\java\Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB33463-676A-4073-A586-1A0BB035A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F300FE3-C753-4ED2-A7E7-E6F2B0B281F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51510C4E-3AE2-48E9-8511-FB6034014CB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C3FF3BE-D8D6-42E1-9386-827C31E975CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Actividad</t>
   </si>
   <si>
-    <t>Tipo de Consumo</t>
-  </si>
-  <si>
-    <t>Unidad</t>
+    <t>Tipo de consumo</t>
   </si>
   <si>
     <t>Valor</t>
@@ -55,70 +52,31 @@
     <t>Periodo de imputacion</t>
   </si>
   <si>
-    <t>Alcance</t>
-  </si>
-  <si>
-    <t>Combustion fija</t>
+    <t>Combustión fija</t>
+  </si>
+  <si>
+    <t>Mensual</t>
+  </si>
+  <si>
+    <t>05/2002</t>
+  </si>
+  <si>
+    <t>Combustión móvil</t>
+  </si>
+  <si>
+    <t>Gasoil</t>
+  </si>
+  <si>
+    <t>Electricidad adquirida y consumida</t>
+  </si>
+  <si>
+    <t>Electricidad</t>
+  </si>
+  <si>
+    <t>Anual</t>
   </si>
   <si>
     <t>Gas Natural</t>
-  </si>
-  <si>
-    <t>m3</t>
-  </si>
-  <si>
-    <t>Mensual</t>
-  </si>
-  <si>
-    <t>02/2020</t>
-  </si>
-  <si>
-    <t>Combustion movil</t>
-  </si>
-  <si>
-    <t>Combustible consumido - Gasoil</t>
-  </si>
-  <si>
-    <t>lts</t>
-  </si>
-  <si>
-    <t>Anual</t>
-  </si>
-  <si>
-    <t>/2021</t>
-  </si>
-  <si>
-    <t>Electricidad adquirida y consumida</t>
-  </si>
-  <si>
-    <t>Electricidad</t>
-  </si>
-  <si>
-    <t>Kwh</t>
-  </si>
-  <si>
-    <t>/2421</t>
-  </si>
-  <si>
-    <t>Nafta</t>
-  </si>
-  <si>
-    <t>lt</t>
-  </si>
-  <si>
-    <t>Materia prima</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Logistica de productos y residuos</t>
-  </si>
-  <si>
-    <t>02/2026</t>
-  </si>
-  <si>
-    <t>Camion de carga</t>
   </si>
 </sst>
 </file>
@@ -154,12 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,22 +428,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D9F111-2FA5-45E2-8986-F34D78041A6B}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB56779-034A-4CD1-B76A-10E0090FDCE9}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,154 +448,61 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>200</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>